<commit_message>
Grade sayfası ve Öğrenci listesi
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sevdaodabas/Desktop/ACU_CSE/projee/CSE311PROJECTT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sevdaodabas/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68063945-D7CF-D447-AE02-E85701D45BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1556067B-0ECE-464F-9786-59829021436C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="920" windowWidth="14000" windowHeight="17100" xr2:uid="{0A591009-2F0C-3046-81C0-F22527DD7B1C}"/>
+    <workbookView xWindow="16020" yWindow="900" windowWidth="14060" windowHeight="16960" xr2:uid="{0A591009-2F0C-3046-81C0-F22527DD7B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,7 +546,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -563,7 +563,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -580,7 +580,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -597,7 +597,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -614,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -631,7 +631,7 @@
         <v>16</v>
       </c>
       <c r="B7">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -648,7 +648,7 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -665,7 +665,7 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -682,7 +682,7 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -699,7 +699,7 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>12345</v>
+        <v>12345678</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
eksik student mailleri eklendi
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sevdaodabas/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sevdaodabas/PycharmProjects/djangofinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1556067B-0ECE-464F-9786-59829021436C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DDA097-6AF5-4D4B-8D17-34F63D7CFD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16020" yWindow="900" windowWidth="14060" windowHeight="16960" xr2:uid="{0A591009-2F0C-3046-81C0-F22527DD7B1C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -141,16 +141,58 @@
   </si>
   <si>
     <t xml:space="preserve">Trabzon </t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>a.yilmaz@live.com</t>
+  </si>
+  <si>
+    <t>a.demir@live.com</t>
+  </si>
+  <si>
+    <t>a.korkmaz@live.com</t>
+  </si>
+  <si>
+    <t>z.durgun@live.com</t>
+  </si>
+  <si>
+    <t>m.gulmez@live.com</t>
+  </si>
+  <si>
+    <t>t.guler@live.com</t>
+  </si>
+  <si>
+    <t>f.agaoglu@live.com</t>
+  </si>
+  <si>
+    <t>s.guclu@live.com</t>
+  </si>
+  <si>
+    <t>h.demirev@live.com</t>
+  </si>
+  <si>
+    <t>m.trabzon@live.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="162"/>
@@ -174,13 +216,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,18 +558,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4758B5-E438-EC4B-BE7E-014E80B53D9A}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +586,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -557,8 +606,11 @@
       <c r="E2">
         <v>220101</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -574,8 +626,11 @@
       <c r="E3">
         <v>220102</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -591,8 +646,11 @@
       <c r="E4">
         <v>220103</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -608,8 +666,11 @@
       <c r="E5">
         <v>220104</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -625,8 +686,11 @@
       <c r="E6">
         <v>220105</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -642,8 +706,11 @@
       <c r="E7">
         <v>220106</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -659,8 +726,11 @@
       <c r="E8">
         <v>220107</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -676,8 +746,11 @@
       <c r="E9">
         <v>220108</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -693,8 +766,11 @@
       <c r="E10">
         <v>220109</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -710,8 +786,24 @@
       <c r="E11">
         <v>2201061</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{0A6CF2BA-5A9A-774B-A451-B25776C9794A}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{26D1558C-A9D0-AE4B-B3A3-3959D651E494}"/>
+    <hyperlink ref="F4:F11" r:id="rId3" display="a.demir@live.com" xr:uid="{8206CBB2-7444-4446-BACE-9BF1A8442036}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{FF0264B8-D27C-2B4D-9743-5A83EAD4B70B}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{454BA94E-A2CB-AA47-95F9-EE43B5A84F69}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{9992B1EC-5ADE-1C47-8DAA-952D2D9BEE2D}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{2529E56B-CC29-D048-B8A1-665DEB290D8C}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{92979465-7210-C440-92B5-5B92E5D2B333}"/>
+    <hyperlink ref="F9" r:id="rId9" xr:uid="{52F116DC-2C0C-1C46-A215-1ECF323724F1}"/>
+    <hyperlink ref="F10" r:id="rId10" xr:uid="{A5BAC968-896D-8742-A328-E7168895200B}"/>
+    <hyperlink ref="F11" r:id="rId11" xr:uid="{443A14DA-61CD-E049-B43C-D503360FD41A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>